<commit_message>
make html-output main branch
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericfoerster/Desktop/torv-reports/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericfoerster/Desktop/torv-reports v4/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D23FD2F-0906-D241-ABFC-AADBE4DE600E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FAB48B-6453-C847-BC4C-58C412AB0580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18100" yWindow="500" windowWidth="22820" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="500" windowWidth="22820" windowHeight="26280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_list" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="1141">
   <si>
     <t>client_number</t>
   </si>
@@ -3411,6 +3411,45 @@
   </si>
   <si>
     <t>DOMINION</t>
+  </si>
+  <si>
+    <t>Adobe Creek National Golf Course</t>
+  </si>
+  <si>
+    <t>Chipeta Golf Course</t>
+  </si>
+  <si>
+    <t>S022</t>
+  </si>
+  <si>
+    <t>Organic Matter % at 440C and Sand Fractions</t>
+  </si>
+  <si>
+    <t>ADOBE</t>
+  </si>
+  <si>
+    <t>CHIPETA</t>
+  </si>
+  <si>
+    <t>BD Landscape Contractors</t>
+  </si>
+  <si>
+    <t>Landscape Art Inc</t>
+  </si>
+  <si>
+    <t>Lanscape</t>
+  </si>
+  <si>
+    <t>BDLAND</t>
+  </si>
+  <si>
+    <t>LANDART</t>
+  </si>
+  <si>
+    <t>Town of Basalt</t>
+  </si>
+  <si>
+    <t>BASALT</t>
   </si>
 </sst>
 </file>
@@ -3980,9 +4019,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4020,7 +4059,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4126,7 +4165,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4268,7 +4307,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4276,10 +4315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4574,6 +4613,46 @@
       </c>
       <c r="B36" t="s">
         <v>1126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>92138</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>92128</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>73293</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>91091</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>46061</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1139</v>
       </c>
     </row>
   </sheetData>
@@ -4591,10 +4670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B614"/>
+  <dimension ref="A1:B615"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B617" sqref="B617"/>
+    <sheetView topLeftCell="A597" workbookViewId="0">
+      <selection activeCell="C621" sqref="C621"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9467,6 +9546,14 @@
       </c>
       <c r="B614" t="s">
         <v>1057</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A615" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B615" t="s">
+        <v>1131</v>
       </c>
     </row>
   </sheetData>
@@ -9695,10 +9782,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8789E2A9-FDC3-4E71-8044-B16DA9DC3A5E}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10170,6 +10257,61 @@
         <v>1072</v>
       </c>
     </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Master database.  Adjusted update-database script to position samples names in correct sample description columns.
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericfoerster/Desktop/torv-reports v4/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FAB48B-6453-C847-BC4C-58C412AB0580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431F96C1-C816-9B46-B966-D32CE08AD626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="500" windowWidth="22820" windowHeight="26280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24200" yWindow="500" windowWidth="22820" windowHeight="26280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_list" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="1147">
   <si>
     <t>client_number</t>
   </si>
@@ -3450,6 +3450,24 @@
   </si>
   <si>
     <t>BASALT</t>
+  </si>
+  <si>
+    <t>Evergro</t>
+  </si>
+  <si>
+    <t>Phillips Lawn Sprinkler Co</t>
+  </si>
+  <si>
+    <t>EVERGRO</t>
+  </si>
+  <si>
+    <t>PHILLIPS</t>
+  </si>
+  <si>
+    <t>Living Earth Dallas</t>
+  </si>
+  <si>
+    <t>LEDALLAS</t>
   </si>
 </sst>
 </file>
@@ -4315,10 +4333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4653,6 +4671,30 @@
       </c>
       <c r="B41" t="s">
         <v>1139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>85137</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>93470</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>74400</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1145</v>
       </c>
     </row>
   </sheetData>
@@ -4672,7 +4714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B615"/>
   <sheetViews>
-    <sheetView topLeftCell="A597" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A580" workbookViewId="0">
       <selection activeCell="C621" sqref="C621"/>
     </sheetView>
   </sheetViews>
@@ -9782,10 +9824,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8789E2A9-FDC3-4E71-8044-B16DA9DC3A5E}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10309,7 +10351,40 @@
         <v>1140</v>
       </c>
       <c r="C47" t="s">
-        <v>1136</v>
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to data and minor changes
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericfoerster/Desktop/torv-reports v4/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericfoerster/Desktop/ torv-reports v4/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431F96C1-C816-9B46-B966-D32CE08AD626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E117CED7-DB35-A24A-A121-29C02F5B7B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24200" yWindow="500" windowWidth="22820" windowHeight="26280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22200" yWindow="500" windowWidth="22820" windowHeight="26280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_list" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="1154">
   <si>
     <t>client_number</t>
   </si>
@@ -3437,9 +3437,6 @@
     <t>Landscape Art Inc</t>
   </si>
   <si>
-    <t>Lanscape</t>
-  </si>
-  <si>
     <t>BDLAND</t>
   </si>
   <si>
@@ -3468,6 +3465,30 @@
   </si>
   <si>
     <t>LEDALLAS</t>
+  </si>
+  <si>
+    <t>Eric George</t>
+  </si>
+  <si>
+    <t>ERICGEORGE</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Turf</t>
+  </si>
+  <si>
+    <t>Crown Mountain Park</t>
+  </si>
+  <si>
+    <t>CROWN</t>
+  </si>
+  <si>
+    <t>William Charles Construction</t>
+  </si>
+  <si>
+    <t>WILLIAM</t>
   </si>
 </sst>
 </file>
@@ -4333,10 +4354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4670,7 +4691,7 @@
         <v>46061</v>
       </c>
       <c r="B41" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -4678,7 +4699,7 @@
         <v>85137</v>
       </c>
       <c r="B42" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -4686,7 +4707,7 @@
         <v>93470</v>
       </c>
       <c r="B43" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -4694,7 +4715,31 @@
         <v>74400</v>
       </c>
       <c r="B44" t="s">
-        <v>1145</v>
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>93769</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>93893</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>94002</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1152</v>
       </c>
     </row>
   </sheetData>
@@ -4714,7 +4759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B615"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A580" workbookViewId="0">
+    <sheetView topLeftCell="A559" workbookViewId="0">
       <selection activeCell="C621" sqref="C621"/>
     </sheetView>
   </sheetViews>
@@ -9824,10 +9869,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8789E2A9-FDC3-4E71-8044-B16DA9DC3A5E}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10326,10 +10371,10 @@
         <v>1134</v>
       </c>
       <c r="B45" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C45" t="s">
-        <v>1136</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -10337,7 +10382,7 @@
         <v>1135</v>
       </c>
       <c r="B46" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="C46" t="s">
         <v>1078</v>
@@ -10345,21 +10390,21 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B47" t="s">
         <v>1139</v>
       </c>
-      <c r="B47" t="s">
-        <v>1140</v>
-      </c>
       <c r="C47" t="s">
-        <v>1078</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B48" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C48" t="s">
         <v>1078</v>
@@ -10367,10 +10412,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B49" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C49" t="s">
         <v>1078</v>
@@ -10378,12 +10423,45 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B50" t="s">
         <v>1145</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>1146</v>
       </c>
-      <c r="C50" t="s">
+      <c r="B51" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C53" t="s">
         <v>1078</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated database and reports
</commit_message>
<xml_diff>
--- a/data/code_book.xlsx
+++ b/data/code_book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericfoerster/Desktop/ torv-reports v4/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E117CED7-DB35-A24A-A121-29C02F5B7B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F1376C-5820-994D-A1AD-D05055FB1FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22200" yWindow="500" windowWidth="22820" windowHeight="26280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13460" yWindow="1040" windowWidth="22820" windowHeight="26280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_list" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="1156">
   <si>
     <t>client_number</t>
   </si>
@@ -3489,6 +3489,12 @@
   </si>
   <si>
     <t>WILLIAM</t>
+  </si>
+  <si>
+    <t>Rifle Creek Golf Course</t>
+  </si>
+  <si>
+    <t>RIFLE</t>
   </si>
 </sst>
 </file>
@@ -4354,10 +4360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4740,6 +4746,14 @@
       </c>
       <c r="B47" t="s">
         <v>1152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>94252</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1154</v>
       </c>
     </row>
   </sheetData>
@@ -9869,10 +9883,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8789E2A9-FDC3-4E71-8044-B16DA9DC3A5E}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10465,6 +10479,17 @@
         <v>1078</v>
       </c>
     </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1072</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>